<commit_message>
resolve the problem ：can't merge bf .xlsx
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15870" windowHeight="7950" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15876" windowHeight="7956" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>Définition</t>
   </si>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2 cartes, pas de couleur,avec la comparaison</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2 cartes, pas de couleur</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -99,10 +95,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2 cartes, avec la couleur et la comparaison</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>v2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -114,10 +106,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v1.3-2ccc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Type</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -174,10 +162,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v1.4-5c13</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Release v3</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -270,6 +254,14 @@
   </si>
   <si>
     <t>Wu, Huang</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.3-5c13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cartes, pas de couleur,avec la comparaison simple</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -451,6 +443,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -459,9 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -889,46 +881,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9" style="13"/>
-    <col min="2" max="2" width="21.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
-    <col min="5" max="5" width="34.125" customWidth="1"/>
-    <col min="7" max="7" width="13.875" customWidth="1"/>
-    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.6328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" customWidth="1"/>
+    <col min="5" max="5" width="34.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -937,13 +929,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>5</v>
@@ -961,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>8</v>
@@ -970,13 +962,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15">
         <v>0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="18">
         <v>43146</v>
@@ -990,26 +982,26 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="10">
-        <f t="shared" ref="A4:A22" si="0">ROW(A4)-2</f>
+        <f t="shared" ref="A4:A21" si="0">ROW(A4)-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="12">
         <v>43152</v>
@@ -1018,7 +1010,7 @@
         <v>43152</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1027,22 +1019,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H5" s="12">
         <v>43153</v>
@@ -1058,71 +1050,71 @@
         <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" s="13" customFormat="1">
       <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" s="13" customFormat="1">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
+      <c r="E8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10">
@@ -1130,95 +1122,95 @@
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="10">
         <v>2</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" s="17" customFormat="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="10">
-        <v>2</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" s="17" customFormat="1">
+      <c r="B10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1">
+      <c r="B11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1230,95 +1222,95 @@
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" s="10">
         <v>3</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" s="13" customFormat="1">
       <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="10">
-        <v>3</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" s="13" customFormat="1">
+      <c r="B14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1">
       <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23" t="s">
+      <c r="B15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1">
+      <c r="C15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="10">
+        <v>4</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" s="10">
         <v>4</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1330,22 +1322,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="D17" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F17" s="10">
         <v>4</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1357,22 +1349,22 @@
         <v>16</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F18" s="10">
         <v>4</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1384,22 +1376,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="10">
         <v>4</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1411,163 +1403,136 @@
         <v>18</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F20" s="10">
         <v>4</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" s="13" customFormat="1">
       <c r="A21" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="10">
-        <v>4</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" s="13" customFormat="1">
-      <c r="A22" s="10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
+      <c r="B21" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="C27" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="C28" s="3" t="s">
-        <v>34</v>
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8">
+        <f>COUNTIFS($F$3,B28,$J$3,"=OK")/COUNTIF($F$3,B28)</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <f>COUNTIFS($F$4:$F$6,B29,$J$4:$J$6,"=OK")/COUNTIF($F$4:$F$6,B29)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="8">
+        <f>COUNTIFS($F$8:$F$9,B30,$J$8:$J$9,"=OK")/COUNTIF($F$8:$F$9,B30)</f>
         <v>0</v>
       </c>
-      <c r="C29" s="8">
-        <f>COUNTIFS($F$3,B29,$J$3,"=OK")/COUNTIF($F$3,B29)</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="B30" s="7">
-        <v>1</v>
-      </c>
-      <c r="C30" s="8">
-        <f>COUNTIFS($F$4:$F$7,B30,$J$4:$J$7,"=OK")/COUNTIF($F$4:$F$7,B30)</f>
-        <v>0.25</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="B31" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="8">
-        <f>COUNTIFS($F$9:$F$10,B31,$J$9:$J$10,"=OK")/COUNTIF($F$9:$F$10,B31)</f>
+        <f>COUNTIFS($F$11:$F$13,B31,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B31)</f>
         <v>0</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="B32" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="8">
-        <f>COUNTIFS($F$12:$F$14,B32,$J$12:$J$14,"=OK")/COUNTIF($F$12:$F$14,B32)</f>
+        <f>COUNTIFS($F$15:$F$20,B32,$J$15:$J$20,"=OK")/COUNTIF($F$15:$F$20,B32)</f>
         <v>0</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="8">
-        <f>COUNTIFS($F$16:$F$21,B33,$J$16:$J$21,"=OK")/COUNTIF($F$16:$F$21,B33)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E14:J14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="G6:G7 G9:G10 G12:G14">
+  <conditionalFormatting sqref="G8:G9 G11:G13 G6">
     <cfRule type="containsText" dxfId="15" priority="23" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:G7 C9:G10 E8 C12:G14 E11 E15 A4:A15 B7:B15 A23:A24 F23:G24 A25:G32 A34:G1048576">
+  <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G13 E10 E14 B6:B14 A22:A23 F22:G23 A24:G31 A33:G1048576 A4:A14">
     <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C32">
+  <conditionalFormatting sqref="C28:C31">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -1598,22 +1563,22 @@
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J5">
+  <conditionalFormatting sqref="J4:J6">
     <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G3 B6:G6">
+  <conditionalFormatting sqref="A1:G3">
     <cfRule type="cellIs" dxfId="11" priority="24" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J3 H6:J7 H9:J10 H12:J14 H23:J32 H34:J1048576">
+  <conditionalFormatting sqref="H1:J3 H8:J9 H11:J13 H22:J31 H33:J1048576 H6:J6">
     <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J6:J7 J9:J10 J12:J14">
+  <conditionalFormatting sqref="J3 J8:J9 J11:J13">
     <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
     </cfRule>
@@ -1628,37 +1593,37 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:G21">
+  <conditionalFormatting sqref="G15:G20">
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:G21">
+  <conditionalFormatting sqref="A15:G20">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16:J21">
+  <conditionalFormatting sqref="H15:J20">
     <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16:J21">
+  <conditionalFormatting sqref="J15:J20">
     <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22 A22:B22">
+  <conditionalFormatting sqref="E21 A21:B21">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:G33">
+  <conditionalFormatting sqref="A32:G32">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C32">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -1684,7 +1649,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:J33">
+  <conditionalFormatting sqref="H32:J32">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -1717,7 +1682,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C29:C32</xm:sqref>
+          <xm:sqref>C28:C31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9CB44186-40AA-4C61-A8C6-EE3F0136660C}">
@@ -1742,7 +1707,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C33</xm:sqref>
+          <xm:sqref>C32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
update the planning form
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28AA7A-97FD-48CB-A9EB-95F29B86079D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416694AA-1F87-4B26-9D78-5ABD9074AE36}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Définition</t>
   </si>
@@ -267,6 +267,22 @@
   </si>
   <si>
     <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HUANG</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -889,7 +905,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1114,7 +1130,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>32</v>
@@ -1125,9 +1141,15 @@
       <c r="G8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="H8" s="12">
+        <v>43165</v>
+      </c>
+      <c r="I8" s="12">
+        <v>43165</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10">
@@ -1141,7 +1163,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>33</v>
@@ -1152,7 +1174,9 @@
       <c r="G9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="12">
+        <v>43165</v>
+      </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
@@ -1187,7 +1211,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>34</v>
@@ -1214,7 +1238,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>35</v>
@@ -1241,7 +1265,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>40</v>
@@ -1491,7 +1515,7 @@
       </c>
       <c r="C30" s="8">
         <f>COUNTIFS($F$8:$F$9,B30,$J$8:$J$9,"=OK")/COUNTIF($F$8:$F$9,B30)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
add test for brelanD
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416694AA-1F87-4B26-9D78-5ABD9074AE36}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F2640E-CA1F-40BD-9AD1-9213B8BAE632}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>Définition</t>
   </si>
@@ -283,6 +283,10 @@
   </si>
   <si>
     <t>HUANG</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -905,7 +909,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1163,7 +1167,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>33</v>
@@ -1177,8 +1181,12 @@
       <c r="H9" s="12">
         <v>43165</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="12">
+        <v>43167</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="17" customFormat="1">
       <c r="A10" s="10">
@@ -1515,7 +1523,7 @@
       </c>
       <c r="C30" s="8">
         <f>COUNTIFS($F$8:$F$9,B30,$J$8:$J$9,"=OK")/COUNTIF($F$8:$F$9,B30)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
update 4card 15value for further development
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nauyn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F2640E-CA1F-40BD-9AD1-9213B8BAE632}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523147A4-2258-48D2-A8AF-5984F3B76422}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Définition</t>
   </si>
@@ -139,22 +139,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v2.1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v2.2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v3.1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v3.2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Original v1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -171,10 +155,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v3.3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>PF</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -287,6 +267,30 @@
   </si>
   <si>
     <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2.1-3c15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2.2-bre</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3.1-4c15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3.2-carre</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v3.3-dp</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -909,7 +913,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -978,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>8</v>
@@ -1047,7 +1051,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -1059,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H5" s="12">
         <v>43153</v>
@@ -1068,7 +1072,7 @@
         <v>43153</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1080,13 +1084,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
@@ -1101,7 +1105,7 @@
         <v>43164</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="13" customFormat="1">
@@ -1109,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="23"/>
@@ -1131,13 +1135,13 @@
         <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10">
         <v>2</v>
@@ -1152,7 +1156,7 @@
         <v>43165</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1164,19 +1168,19 @@
         <v>25</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="F9" s="10">
         <v>2</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H9" s="12">
         <v>43165</v>
@@ -1185,7 +1189,7 @@
         <v>43167</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="17" customFormat="1">
@@ -1194,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="23"/>
@@ -1216,13 +1220,13 @@
         <v>25</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
@@ -1230,9 +1234,15 @@
       <c r="G11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="H11" s="12">
+        <v>43167</v>
+      </c>
+      <c r="I11" s="12">
+        <v>43167</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="10">
@@ -1243,13 +1253,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -1273,16 +1283,16 @@
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="F13" s="10">
         <v>3</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -1294,7 +1304,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
@@ -1316,13 +1326,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F15" s="10">
         <v>4</v>
@@ -1346,10 +1356,10 @@
         <v>27</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" s="10">
         <v>4</v>
@@ -1373,16 +1383,16 @@
         <v>28</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F17" s="10">
         <v>4</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1397,19 +1407,19 @@
         <v>25</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F18" s="10">
         <v>4</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1427,16 +1437,16 @@
         <v>29</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F19" s="10">
         <v>4</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1454,16 +1464,16 @@
         <v>30</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="10">
         <v>4</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1475,12 +1485,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
       <c r="E21" s="24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
@@ -1535,7 +1545,7 @@
       </c>
       <c r="C31" s="8">
         <f>COUNTIFS($F$11:$F$13,B31,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B31)</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>22</v>
@@ -1550,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the fonction of regle two paires
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nauyn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523147A4-2258-48D2-A8AF-5984F3B76422}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17E73B-2DA2-4F07-A3CE-CC54B01412D7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Définition</t>
   </si>
@@ -291,6 +291,10 @@
   </si>
   <si>
     <t>v3.3-dp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -913,7 +917,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1294,9 +1298,15 @@
       <c r="G13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="H13" s="12">
+        <v>43167</v>
+      </c>
+      <c r="I13" s="12">
+        <v>43167</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1">
       <c r="A14" s="10">
@@ -1545,7 +1555,7 @@
       </c>
       <c r="C31" s="8">
         <f>COUNTIFS($F$11:$F$13,B31,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B31)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Add regle Carre and already tested
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -221,8 +221,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -247,6 +247,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="DengXian"/>
@@ -255,7 +263,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,33 +330,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -306,23 +352,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="DengXian"/>
       <charset val="134"/>
@@ -337,47 +376,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,43 +430,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,13 +586,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,121 +604,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,36 +676,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -719,17 +689,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -750,11 +709,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -773,16 +753,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -791,133 +791,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1719,7 +1719,9 @@
       <c r="I13" s="17">
         <v>43167</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:10">
       <c r="A14" s="7">
@@ -1968,7 +1970,7 @@
       </c>
       <c r="C31" s="24">
         <f>COUNTIFS($F$11:$F$13,B31,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B31)</f>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>45</v>
@@ -1999,33 +2001,13 @@
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:J21"/>
   </mergeCells>
-  <conditionalFormatting sqref="A12:G12">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="containsText" dxfId="1" priority="4" operator="between" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:J12">
+  <conditionalFormatting sqref="A32:G32">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="between" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:G32">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2033,11 +2015,11 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{fa1ee209-d01e-4f6c-b023-79a9d0bdfa02}</x14:id>
+          <x14:id>{ef6dc489-049b-4793-8e64-a04bd08c7ad3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2045,18 +2027,18 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b06e53d3-7aff-475b-9c02-6ccb011bc46c}</x14:id>
+          <x14:id>{a69179d7-6d61-4aea-9a98-27dfb61f524a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:J32">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2064,11 +2046,11 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e37c6bfd-82ab-4de1-9701-45b95d7a7b26}</x14:id>
+          <x14:id>{31c186c7-7681-48f1-a3b9-a67ba649f046}</x14:id>
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2076,78 +2058,78 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0125efa4-a9a5-416b-b39f-e5a5fd05436e}</x14:id>
+          <x14:id>{15a8883c-69a5-45ce-acb2-c1a75cbc9840}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule type="containsText" dxfId="1" priority="22" operator="between" text="PF">
+    <cfRule type="containsText" dxfId="1" priority="18" operator="between" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G20">
-    <cfRule type="containsText" dxfId="1" priority="13" operator="between" text="PF">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="between" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J6">
-    <cfRule type="containsText" dxfId="2" priority="20" operator="between" text="NOK">
+    <cfRule type="containsText" dxfId="2" priority="16" operator="between" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J20">
-    <cfRule type="containsText" dxfId="2" priority="11" operator="between" text="NOK">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="between" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G3">
-    <cfRule type="cellIs" dxfId="0" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J3 H8:J9 H11:J11 H33:J1048576 H6:J6 H22:J23 H25:J31 H13:J13">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
+  <conditionalFormatting sqref="H1:J3 H8:J9 H11:J13 H33:J1048576 H6:J6 H22:J22 H24:J31">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J8:J9 J11 J13">
-    <cfRule type="containsText" dxfId="2" priority="24" operator="between" text="NOK">
+  <conditionalFormatting sqref="J3 J8:J9 J11:J13">
+    <cfRule type="containsText" dxfId="2" priority="20" operator="between" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G11 A4:A11 A33:G1048576 E10 E14 B6:B11 A14:B14 A25:G31 F22:G23 A22:A23 A13:G13">
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
+  <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G12 A24:G31 A4:A11 E10 E14 B6:B11 A12:B12 A14:B14 F22:G22 A22 A33:G1048576 A13:G13">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G5">
-    <cfRule type="cellIs" dxfId="0" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J5">
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G9 G11 G6 G13">
-    <cfRule type="containsText" dxfId="1" priority="27" operator="between" text="PF">
+  <conditionalFormatting sqref="G8:G9 G11:G13 G6">
+    <cfRule type="containsText" dxfId="1" priority="23" operator="between" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:G20">
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J20">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21 A21:B21">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2158,7 +2140,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{fa1ee209-d01e-4f6c-b023-79a9d0bdfa02}">
+          <x14:cfRule type="dataBar" id="{ef6dc489-049b-4793-8e64-a04bd08c7ad3}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2170,7 +2152,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{b06e53d3-7aff-475b-9c02-6ccb011bc46c}">
+          <x14:cfRule type="dataBar" id="{a69179d7-6d61-4aea-9a98-27dfb61f524a}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2183,7 +2165,7 @@
           <xm:sqref>C32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e37c6bfd-82ab-4de1-9701-45b95d7a7b26}">
+          <x14:cfRule type="dataBar" id="{31c186c7-7681-48f1-a3b9-a67ba649f046}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2195,7 +2177,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{0125efa4-a9a5-416b-b39f-e5a5fd05436e}">
+          <x14:cfRule type="dataBar" id="{15a8883c-69a5-45ce-acb2-c1a75cbc9840}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Add regle Suite and already tested
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3E6B0-3260-412B-A7D7-F9469963F400}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="15870" windowHeight="7950" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15870" windowHeight="7950" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>Définition</t>
   </si>
@@ -200,19 +206,17 @@
   </si>
   <si>
     <t>Avancement des releases</t>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,151 +239,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="DengXian"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,7 +260,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505"/>
+        <fgColor theme="0" tint="-0.14993743705557422"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,7 +272,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.349986266670736"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,194 +282,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -663,251 +343,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -919,9 +357,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -946,13 +381,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -962,60 +390,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1037,9 +447,113 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1048,6 +562,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1305,16 +822,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1330,679 +847,682 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:10">
-      <c r="A3" s="7">
+    <row r="3" spans="1:10" s="1" customFormat="1">
+      <c r="A3" s="6">
         <f>ROW(A3)-2</f>
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <v>0</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>43146</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>43150</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <f t="shared" ref="A4:A21" si="0">ROW(A4)-2</f>
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>43152</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <v>43152</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <v>43153</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="16">
         <v>43153</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="16">
         <v>43160</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <v>43164</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:10">
-      <c r="A7" s="7">
+    <row r="7" spans="1:10" s="1" customFormat="1">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>43165</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>43165</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>2</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="16">
         <v>43165</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="16">
         <v>43167</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" spans="1:10">
-      <c r="A10" s="7">
+    <row r="10" spans="1:10" s="2" customFormat="1">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" s="3" customFormat="1" spans="1:10">
-      <c r="A11" s="7">
+    <row r="11" spans="1:10" s="3" customFormat="1">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>3</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="16">
         <v>43167</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="16">
         <v>43167</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>3</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="16">
         <v>43167</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="16">
         <v>43167</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>3</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <v>43167</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <v>43167</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:10">
-      <c r="A14" s="7">
+    <row r="14" spans="1:10" s="1" customFormat="1">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="26"/>
     </row>
-    <row r="15" s="3" customFormat="1" spans="1:10">
-      <c r="A15" s="7">
+    <row r="15" spans="1:10" s="3" customFormat="1">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>4</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="16">
         <v>43167</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <v>43167</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>4</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>43168</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <v>43168</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>4</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="16">
         <v>43167</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>4</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>4</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>4</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:10">
-      <c r="A21" s="7">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21" t="s">
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
       <c r="J21" s="26"/>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="1:10">
       <c r="C27" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="23">
+    <row r="28" spans="1:10">
+      <c r="B28" s="17">
         <v>0</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="18">
         <f>COUNTIFS($F$3,B28,$J$3,"=OK")/COUNTIF($F$3,B28)</f>
         <v>1</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="23">
+    <row r="29" spans="1:10">
+      <c r="B29" s="17">
         <v>1</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="18">
         <f>COUNTIFS($F$4:$F$6,B29,$J$4:$J$6,"=OK")/COUNTIF($F$4:$F$6,B29)</f>
         <v>1</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="1:10">
       <c r="B30" s="4">
         <v>2</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="18">
         <f>COUNTIFS($F$8:$F$9,B30,$J$8:$J$9,"=OK")/COUNTIF($F$8:$F$9,B30)</f>
         <v>1</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="1:10">
       <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="18">
         <f>COUNTIFS($F$11:$F$13,B31,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B31)</f>
         <v>1</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="1:10">
       <c r="B32" s="4">
         <v>4</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="18">
         <f>COUNTIFS($F$15:$F$20,B32,$J$15:$J$20,"=OK")/COUNTIF($F$15:$F$20,B32)</f>
-        <v>0.166666666666667</v>
-      </c>
-      <c r="D32" s="25" t="s">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:J21"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:J10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:J21"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A32:G32">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2015,7 +1535,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8f2b341f-4b4c-4b52-9f8f-0e033bbd43a4}</x14:id>
+          <x14:id>{8F2B341F-4B4C-4B52-9F8F-0E033BBD43A4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2027,13 +1547,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{38c55fad-70f3-4370-8194-15c92885ccc8}</x14:id>
+          <x14:id>{38C55FAD-70F3-4370-8194-15C92885CCC8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:J32">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2046,7 +1566,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bb8b9df7-91f1-4b9b-b382-2bf122cc4134}</x14:id>
+          <x14:id>{BB8B9DF7-91F1-4B9B-B382-2BF122CC4134}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2058,73 +1578,73 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{705825eb-c340-4cfb-9ded-853ffcdfc2c3}</x14:id>
+          <x14:id>{705825EB-C340-4CFB-9DED-853FFCDFC2C3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule type="containsText" dxfId="1" priority="18" operator="between" text="PF">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G20">
-    <cfRule type="containsText" dxfId="1" priority="9" operator="between" text="PF">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J6">
-    <cfRule type="containsText" dxfId="2" priority="16" operator="between" text="NOK">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J20">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="between" text="NOK">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G3">
-    <cfRule type="cellIs" dxfId="0" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="24" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3 H8:J9 H11:J13 H22:J31 H33:J1048576 H6:J6">
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3 J8:J9 J11:J13">
-    <cfRule type="containsText" dxfId="2" priority="20" operator="between" text="NOK">
+    <cfRule type="containsText" dxfId="7" priority="20" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G13 E10 E14 B6:B14 A22:A23 F22:G23 A24:G31 A33:G1048576 A4:A14">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G5">
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="19" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J5">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G9 G11:G13 G6">
-    <cfRule type="containsText" dxfId="1" priority="23" operator="between" text="PF">
+    <cfRule type="containsText" dxfId="3" priority="23" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:G20">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J20">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2133,14 +1653,13 @@
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8f2b341f-4b4c-4b52-9f8f-0e033bbd43a4}">
+          <x14:cfRule type="dataBar" id="{8F2B341F-4B4C-4B52-9F8F-0E033BBD43A4}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2152,7 +1671,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{38c55fad-70f3-4370-8194-15c92885ccc8}">
+          <x14:cfRule type="dataBar" id="{38C55FAD-70F3-4370-8194-15C92885CCC8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2165,7 +1684,7 @@
           <xm:sqref>C32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bb8b9df7-91f1-4b9b-b382-2bf122cc4134}">
+          <x14:cfRule type="dataBar" id="{BB8B9DF7-91F1-4B9B-B382-2BF122CC4134}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2177,7 +1696,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{705825eb-c340-4cfb-9ded-853ffcdfc2c3}">
+          <x14:cfRule type="dataBar" id="{705825EB-C340-4CFB-9DED-853FFCDFC2C3}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Update  the spec (version 5.2)
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2049D3-F1FA-48C7-B5CA-BD1A0D557424}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38E5196-3015-4ABA-A325-8051A018618E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15876" windowHeight="7956" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>Définition</t>
   </si>
@@ -220,19 +220,31 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v5.1</t>
+    <t>OK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v5.2</t>
+    <t>OK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>v5.3</t>
+    <t>Liu</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>OK</t>
+    <t>Wu</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v5.1-4c</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v5.2-couleur</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v5.3-qf</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -884,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -1434,7 +1446,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F19" s="6">
         <v>5</v>
@@ -1449,7 +1461,7 @@
         <v>43173</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1464,10 +1476,10 @@
         <v>54</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F20" s="6">
         <v>5</v>
@@ -1475,9 +1487,15 @@
       <c r="G20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="H20" s="16">
+        <v>43173</v>
+      </c>
+      <c r="I20" s="16">
+        <v>43173</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6">
@@ -1491,10 +1509,10 @@
         <v>55</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F21" s="6">
         <v>5</v>
@@ -1596,7 +1614,7 @@
       </c>
       <c r="C34" s="18">
         <f>COUNTIFS($F$19:$F$21,B34,$J$19:$J$21,"=OK")/COUNTIF($F$19:$F$21,B34)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
add new regle flush and tested
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38E5196-3015-4ABA-A325-8051A018618E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D13FF-344B-4242-855A-7AAA87D2C8D2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15876" windowHeight="7956" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>Définition</t>
   </si>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -1520,9 +1520,15 @@
       <c r="G21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="H21" s="16">
+        <v>43173</v>
+      </c>
+      <c r="I21" s="16">
+        <v>43173</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1">
       <c r="A22" s="6">
@@ -1614,7 +1620,7 @@
       </c>
       <c r="C34" s="18">
         <f>COUNTIFS($F$19:$F$21,B34,$J$19:$J$21,"=OK")/COUNTIF($F$19:$F$21,B34)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
corriger des erruers dans le tableau
</commit_message>
<xml_diff>
--- a/A-specs.xlsx
+++ b/A-specs.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-space\poker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D13FF-344B-4242-855A-7AAA87D2C8D2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15876" windowHeight="7956" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
   <si>
     <t>Définition</t>
   </si>
@@ -106,7 +100,7 @@
     <t>v2</t>
   </si>
   <si>
-    <t xml:space="preserve">3 cartes avec 15 valeur        </t>
+    <t xml:space="preserve">3 cartes avec 15 valeurs        </t>
   </si>
   <si>
     <t>Wu</t>
@@ -130,7 +124,7 @@
     <t>v3</t>
   </si>
   <si>
-    <t>4 cartes avec 15 valeur</t>
+    <t>4 cartes avec 15 valeurs</t>
   </si>
   <si>
     <t>HUANG</t>
@@ -160,7 +154,7 @@
     <t>v4</t>
   </si>
   <si>
-    <t>5 carte avec 15 valeur, ajouter le judger qui 'return max point'</t>
+    <t>5 cartes avec 15 valeurs, ajouter le judger qui 'return max point'</t>
   </si>
   <si>
     <t>Huang</t>
@@ -181,78 +175,50 @@
     <t>v4.3-full</t>
   </si>
   <si>
-    <t>5 carte avec 15 valeur avec couleur</t>
+    <t>Release v5</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>5 cartes avec 15 valeurs avec couleur</t>
+  </si>
+  <si>
+    <t>v5.1-4c</t>
   </si>
   <si>
     <t>ajouter regle: Couleur</t>
   </si>
   <si>
+    <t>v5.2-couleur</t>
+  </si>
+  <si>
     <t>ajouter regle: Quinte Flush</t>
   </si>
   <si>
-    <t>v5</t>
+    <t>v5.3-qf</t>
+  </si>
+  <si>
+    <t>Release v6</t>
+  </si>
+  <si>
+    <t>v6</t>
   </si>
   <si>
     <t>Avancement des releases</t>
-  </si>
-  <si>
-    <t>OK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release v5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release v6</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v6</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wu</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v5.1-4c</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v5.2-couleur</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>v5.3-qf</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,13 +241,158 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,7 +407,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14993743705557422"/>
+        <fgColor theme="0" tint="-0.149937437055574"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.349986266670736"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,8 +429,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -379,9 +676,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -394,6 +933,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -417,15 +959,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -433,65 +966,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -513,113 +1050,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -628,9 +1061,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -888,717 +1318,717 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="21.36328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="59.6328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="5" max="5" width="34.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.3666666666667" style="4" customWidth="1"/>
+    <col min="3" max="3" width="59.6333333333333" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.9083333333333" customWidth="1"/>
+    <col min="5" max="5" width="34.0916666666667" customWidth="1"/>
+    <col min="7" max="7" width="13.9083333333333" customWidth="1"/>
+    <col min="8" max="8" width="12.6333333333333" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1">
-      <c r="A3" s="6">
+    <row r="3" s="1" customFormat="1" spans="1:10">
+      <c r="A3" s="7">
         <f>ROW(A3)-2</f>
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="13">
         <v>0</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="14">
         <v>43146</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="14">
         <v>43150</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <f t="shared" ref="A4:A22" si="0">ROW(A4)-2</f>
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="17">
         <v>43152</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="17">
         <v>43152</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="17">
         <v>43153</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="17">
         <v>43153</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="17">
         <v>43160</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="17">
         <v>43164</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1">
-      <c r="A7" s="6">
+    <row r="7" s="1" customFormat="1" spans="1:10">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="25"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="17">
         <v>43165</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="17">
         <v>43165</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="17">
         <v>43165</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="17">
         <v>43167</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1">
-      <c r="A10" s="6">
+    <row r="10" s="2" customFormat="1" spans="1:10">
+      <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1">
-      <c r="A11" s="6">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" s="3" customFormat="1" spans="1:10">
+      <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="17">
         <v>43167</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="17">
         <v>43167</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <v>3</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="17">
         <v>43167</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="17">
         <v>43167</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <v>3</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="17">
         <v>43167</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="17">
         <v>43167</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1">
-      <c r="A14" s="6">
+    <row r="14" s="1" customFormat="1" spans="1:10">
+      <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1">
-      <c r="A15" s="6">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:10">
+      <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="7">
         <v>4</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="16">
+      <c r="G15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="17">
         <v>43167</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="17">
         <v>43167</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="7">
         <v>4</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="17">
         <v>43168</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="17">
         <v>43168</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>58</v>
+      <c r="J16" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="6">
+      <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="7">
         <v>4</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="17">
         <v>43167</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="17">
         <v>43169</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1">
-      <c r="A18" s="6">
+      <c r="J17" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:10">
+      <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="B18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="6">
+      <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="E19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="7">
         <v>5</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="17">
         <v>43169</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="17">
         <v>43173</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>64</v>
+      <c r="J19" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="6">
+      <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="C20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="7">
         <v>5</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="17">
         <v>43173</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="17">
         <v>43173</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>65</v>
+      <c r="J20" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="C21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="7">
         <v>5</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="17">
         <v>43173</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="17">
         <v>43173</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1">
-      <c r="A22" s="6">
+      <c r="J21" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:10">
+      <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="C28" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="B29" s="17">
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="23">
         <v>0</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="24">
         <f>COUNTIFS($F$3,B29,$J$3,"=OK")/COUNTIF($F$3,B29)</f>
         <v>1</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="B30" s="17">
+    <row r="30" spans="2:4">
+      <c r="B30" s="23">
         <v>1</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="24">
         <f>COUNTIFS($F$4:$F$6,B30,$J$4:$J$6,"=OK")/COUNTIF($F$4:$F$6,B30)</f>
         <v>1</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="2:4">
       <c r="B31" s="4">
         <v>2</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="24">
         <f>COUNTIFS($F$8:$F$9,B31,$J$8:$J$9,"=OK")/COUNTIF($F$8:$F$9,B31)</f>
         <v>1</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="2:4">
       <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="24">
         <f>COUNTIFS($F$11:$F$13,B32,$J$11:$J$13,"=OK")/COUNTIF($F$11:$F$13,B32)</f>
         <v>1</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="25" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1606,44 +2036,43 @@
       <c r="B33" s="4">
         <v>4</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="24">
         <f>COUNTIFS($F$15:$F$17,B33,$J$15:$J$17,"=OK")/COUNTIF($F$15:$F$17,B33)</f>
         <v>1</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>56</v>
+      <c r="D33" s="25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="4">
         <v>5</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="24">
         <f>COUNTIFS($F$19:$F$21,B34,$J$19:$J$21,"=OK")/COUNTIF($F$19:$F$21,B34)</f>
         <v>1</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>63</v>
+      <c r="D34" s="25" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:J22"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:J10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:J14"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:J18"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:J22"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A33:G33">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1656,7 +2085,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8F2B341F-4B4C-4B52-9F8F-0E033BBD43A4}</x14:id>
+          <x14:id>{58d541bc-1a56-4685-9f29-121f225d8637}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1668,13 +2097,49 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{38C55FAD-70F3-4370-8194-15C92885CCC8}</x14:id>
+          <x14:id>{6292bd84-0a37-447d-9510-55a39993423a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:J33">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:G34">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{12811b4f-8337-4cbd-9be3-9c13d27743df}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{81e5c798-67aa-45e4-a3b6-7696e39bfb09}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:J34">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1687,7 +2152,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BB8B9DF7-91F1-4B9B-B382-2BF122CC4134}</x14:id>
+          <x14:id>{15991765-07cc-4928-800f-9cee65a91b84}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1699,129 +2164,94 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{705825EB-C340-4CFB-9DED-853FFCDFC2C3}</x14:id>
+          <x14:id>{a12c1d4e-6b96-4795-acef-90113453e0eb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="1" priority="23" operator="between" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J6">
+    <cfRule type="containsText" dxfId="2" priority="21" operator="between" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:G3">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J3 H8:J9 H11:J13 H23:J32 H35:J1048576 H6:J6">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3 J8:J9 J11:J13">
+    <cfRule type="containsText" dxfId="2" priority="25" operator="between" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G13 E10 E14 B6:B14 A23:A24 F23:G24 A25:G32 A35:G1048576 A4:A14">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G5">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J5">
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G9 G11:G13 G6">
+    <cfRule type="containsText" dxfId="1" priority="28" operator="between" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:G17 A19:G21">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+      <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G17 G19:G21">
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="1" priority="14" operator="between" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J6">
-    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
+  <conditionalFormatting sqref="H15:J17 H19:J21">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+      <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J17 J19:J21">
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="2" priority="12" operator="between" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G3">
-    <cfRule type="cellIs" dxfId="12" priority="29" operator="equal">
+  <conditionalFormatting sqref="E18 A18:B18">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J3 H8:J9 H11:J13 H23:J32 H35:J1048576 H6:J6">
-    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J8:J9 J11:J13">
-    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:G6 C8:G9 E7 C11:G13 E10 E14 B6:B14 A23:A24 F23:G24 A25:G32 A35:G1048576 A4:A14">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:G5">
-    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:J5">
-    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G9 G11:G13 G6">
-    <cfRule type="containsText" dxfId="6" priority="28" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:G17 A19:G21">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:J17 H19:J21">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
-      <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22 A22:B22">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18 A18:B18">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34:G34">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0B5F63E7-C216-411F-8831-469A069CBF06}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C4450398-56B3-4014-A800-B580BEAF60DB}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34:J34">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8F2B341F-4B4C-4B52-9F8F-0E033BBD43A4}">
+          <x14:cfRule type="dataBar" id="{58d541bc-1a56-4685-9f29-121f225d8637}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -1833,7 +2263,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{38C55FAD-70F3-4370-8194-15C92885CCC8}">
+          <x14:cfRule type="dataBar" id="{6292bd84-0a37-447d-9510-55a39993423a}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1846,7 +2276,7 @@
           <xm:sqref>C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BB8B9DF7-91F1-4B9B-B382-2BF122CC4134}">
+          <x14:cfRule type="dataBar" id="{12811b4f-8337-4cbd-9be3-9c13d27743df}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -1858,7 +2288,32 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{705825EB-C340-4CFB-9DED-853FFCDFC2C3}">
+          <x14:cfRule type="dataBar" id="{81e5c798-67aa-45e4-a3b6-7696e39bfb09}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{15991765-07cc-4928-800f-9cee65a91b84}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{a12c1d4e-6b96-4795-acef-90113453e0eb}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1870,31 +2325,6 @@
           </x14:cfRule>
           <xm:sqref>C29:C32</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0B5F63E7-C216-411F-8831-469A069CBF06}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{C4450398-56B3-4014-A800-B580BEAF60DB}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C34</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>